<commit_message>
Adding ingest rake task, and version validations
</commit_message>
<xml_diff>
--- a/digital_cicognara_template.xlsx
+++ b/digital_cicognara_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="30820" yWindow="-2980" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>digital_cico_number</t>
   </si>
@@ -42,12 +42,6 @@
     <t>other_number</t>
   </si>
   <si>
-    <t>edition_statement</t>
-  </si>
-  <si>
-    <t>publication_statement</t>
-  </si>
-  <si>
     <t>additional_responsibility</t>
   </si>
   <si>
@@ -61,18 +55,38 @@
   </si>
   <si>
     <t>based_on_original</t>
+  </si>
+  <si>
+    <t>version_edition_statement</t>
+  </si>
+  <si>
+    <t>version_publication_statement</t>
+  </si>
+  <si>
+    <t>version_publication_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,13 +106,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,13 +447,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,25 +476,28 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>